<commit_message>
更新错误代码 Signed-off-by: moyilong <moyilong@foxmail.com>
</commit_message>
<xml_diff>
--- a/sys/kernel/Doc/错误代码.xlsx
+++ b/sys/kernel/Doc/错误代码.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="147">
   <si>
     <t>代码</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -577,6 +577,29 @@
   </si>
   <si>
     <t>内核-init</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0xaff221f9</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>APP-Initer发现一个PPK模块</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>提示</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>内核-App</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">0xaff221fa </t>
+  </si>
+  <si>
+    <t>APP-Initer发现一个EXT模块</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -957,10 +980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36:D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1526,6 +1549,34 @@
       </c>
       <c r="D34" t="s">
         <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>141</v>
+      </c>
+      <c r="B35" t="s">
+        <v>142</v>
+      </c>
+      <c r="C35" t="s">
+        <v>143</v>
+      </c>
+      <c r="D35" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>145</v>
+      </c>
+      <c r="B36" t="s">
+        <v>146</v>
+      </c>
+      <c r="C36" t="s">
+        <v>143</v>
+      </c>
+      <c r="D36" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>